<commit_message>
Modify deck to go up to 2055
</commit_message>
<xml_diff>
--- a/CreateBaseDeck/ExcelUserData/UserData.xlsx
+++ b/CreateBaseDeck/ExcelUserData/UserData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Remote\Desktop\Projects\TemoaHurricane_OEA\TEMOA_GIT\TemoaHurricane_V2\CreateBaseDeck\ExcelUserData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEDABAAC-6A29-421A-81DF-7B1DE8C72912}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{893DB414-FFFD-4D1E-9FBD-D4BA7590FA60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="839" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="839" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="technologies" sheetId="1" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3217" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3221" uniqueCount="376">
   <si>
     <t>tech</t>
   </si>
@@ -2965,7 +2965,7 @@
   <dimension ref="A1:E57"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2:A57"/>
     </sheetView>
   </sheetViews>
@@ -3838,7 +3838,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4301,8 +4301,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBE0BB4B-A87E-47DE-8321-0EFAC4350DE2}">
   <dimension ref="A1:H52"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5106,7 +5106,7 @@
         <v>31</v>
       </c>
       <c r="G36">
-        <f t="shared" si="1"/>
+        <f>G35*(100+$B$52)/100</f>
         <v>691.20782307077172</v>
       </c>
       <c r="H36">
@@ -5125,6 +5125,16 @@
       <c r="C37">
         <v>2025</v>
       </c>
+      <c r="F37" t="s">
+        <v>31</v>
+      </c>
+      <c r="G37">
+        <f>G36*(100+$B$52)/100</f>
+        <v>698.13805197447482</v>
+      </c>
+      <c r="H37">
+        <v>2054</v>
+      </c>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="3">
@@ -5137,6 +5147,16 @@
       </c>
       <c r="C38">
         <v>2026</v>
+      </c>
+      <c r="F38" t="s">
+        <v>31</v>
+      </c>
+      <c r="G38">
+        <f>G37*(100+$B$52)/100</f>
+        <v>705.13776515056986</v>
+      </c>
+      <c r="H38">
+        <v>2055</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -5806,7 +5826,7 @@
   <dimension ref="A1:E61"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
@@ -16714,9 +16734,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96CB1107-551A-4401-A108-C4996FB8D590}">
   <dimension ref="A1:AI90"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A90" sqref="A2:A90"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AJ1" sqref="AJ1:AO1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -26370,9 +26390,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CD5D24F-D6D8-45F0-9B18-7F7BBE5186DB}">
   <dimension ref="A1:AI119"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K43" sqref="K43"/>
+      <selection pane="bottomLeft" activeCell="AJ1" sqref="AJ1:AO1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -39129,9 +39149,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1F64963-0CDD-4BE6-B0AC-E6FD0D7CCBEC}">
   <dimension ref="A1:AI119"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A85" sqref="A85:C87"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AJ1" sqref="AJ1:AQ1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -52010,10 +52030,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{465044A0-2557-4FC4-8230-2D5F5E941F36}">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -52609,6 +52629,40 @@
         <v>2053</v>
       </c>
       <c r="D35" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" t="str">
+        <f>DemandCalculations!F37</f>
+        <v>NC</v>
+      </c>
+      <c r="B36">
+        <f>DemandCalculations!G37</f>
+        <v>698.13805197447482</v>
+      </c>
+      <c r="C36">
+        <f>DemandCalculations!H37</f>
+        <v>2054</v>
+      </c>
+      <c r="D36" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" t="str">
+        <f>DemandCalculations!F38</f>
+        <v>NC</v>
+      </c>
+      <c r="B37">
+        <f>DemandCalculations!G38</f>
+        <v>705.13776515056986</v>
+      </c>
+      <c r="C37">
+        <f>DemandCalculations!H38</f>
+        <v>2055</v>
+      </c>
+      <c r="D37" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Define Transmission Inter regions
</commit_message>
<xml_diff>
--- a/CreateBaseDeck/ExcelUserData/UserData.xlsx
+++ b/CreateBaseDeck/ExcelUserData/UserData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Remote\Desktop\Projects\TemoaHurricane_OEA\TEMOA_GIT\TemoaHurricane_V2\CreateBaseDeck\ExcelUserData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{893DB414-FFFD-4D1E-9FBD-D4BA7590FA60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C607748C-F948-43A3-B550-BE7D2D0AA4CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="839" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7320" yWindow="2160" windowWidth="21600" windowHeight="11385" tabRatio="935" firstSheet="3" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="technologies" sheetId="1" r:id="rId1"/>
@@ -25,6 +25,7 @@
     <sheet name="ReadMe" sheetId="12" r:id="rId10"/>
     <sheet name="HydroPlantsNC" sheetId="13" r:id="rId11"/>
     <sheet name="DemandCalculations" sheetId="3" r:id="rId12"/>
+    <sheet name="Transmission" sheetId="18" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -69,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3221" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3228" uniqueCount="383">
   <si>
     <t>tech</t>
   </si>
@@ -1208,6 +1209,27 @@
   </si>
   <si>
     <t>cost_fixed_notes</t>
+  </si>
+  <si>
+    <t>Voltage</t>
+  </si>
+  <si>
+    <t>Percentage of Transmission Voltages from Duke (https://starw1.ncuc.gov/NCUC/ViewFile.aspx?Id=1b035aef-cdb1-4a8a-ae0c-599d02ab61cf)</t>
+  </si>
+  <si>
+    <t>Total Miles DEP+DEC</t>
+  </si>
+  <si>
+    <t>Percentage of Total Miles</t>
+  </si>
+  <si>
+    <t>Transmission Investment Cost From ReEDS (ReEDS_OpenAccess/inputs/transmission/rev_transmission_basecost.csv) converted from 2004 to 2022 values (x1.55)</t>
+  </si>
+  <si>
+    <t>Investment Cost [$/MW-Mile]</t>
+  </si>
+  <si>
+    <t>Average Transmission Cost  [$/MW-Mile]</t>
   </si>
 </sst>
 </file>
@@ -4826,7 +4848,7 @@
         <v>31</v>
       </c>
       <c r="G23">
-        <f t="shared" ref="G23:G36" si="1">G22*(100+$B$52)/100</f>
+        <f t="shared" ref="G23:G35" si="1">G22*(100+$B$52)/100</f>
         <v>607.13322443722291</v>
       </c>
       <c r="H23">
@@ -5317,6 +5339,149 @@
     <mergeCell ref="F1:H1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F425B7AA-21D1-411D-A9AF-54EA873F398D}">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" customWidth="1"/>
+    <col min="4" max="4" width="24" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>376</v>
+      </c>
+      <c r="B4" t="s">
+        <v>381</v>
+      </c>
+      <c r="C4" t="s">
+        <v>378</v>
+      </c>
+      <c r="D4" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5">
+        <v>69</v>
+      </c>
+      <c r="B5">
+        <f>5941.27*1.55</f>
+        <v>9208.9685000000009</v>
+      </c>
+      <c r="C5">
+        <v>133</v>
+      </c>
+      <c r="D5">
+        <f>C5/SUM($C$5:$C$8)</f>
+        <v>8.057187859695886E-3</v>
+      </c>
+      <c r="E5">
+        <f>B5*C5/1000</f>
+        <v>1224.7928105000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6">
+        <v>138</v>
+      </c>
+      <c r="B6">
+        <f>3553.52*1.55</f>
+        <v>5507.9560000000001</v>
+      </c>
+      <c r="C6">
+        <v>9417</v>
+      </c>
+      <c r="D6">
+        <f t="shared" ref="D6:D8" si="0">C6/SUM($C$5:$C$8)</f>
+        <v>0.57048524868237716</v>
+      </c>
+      <c r="E6">
+        <f t="shared" ref="E6:E8" si="1">B6*C6/1000</f>
+        <v>51868.421652000005</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7">
+        <v>230</v>
+      </c>
+      <c r="B7">
+        <f>2900.44*1.55</f>
+        <v>4495.6819999999998</v>
+      </c>
+      <c r="C7">
+        <v>6089</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>0.36887381111043799</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>27374.207697999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8">
+        <v>500</v>
+      </c>
+      <c r="B8">
+        <f>2001.36*1.55</f>
+        <v>3102.1079999999997</v>
+      </c>
+      <c r="C8">
+        <v>868</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>5.2583752347488945E-2</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>2692.6297439999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="E9">
+        <f>SUM(E5:E8)</f>
+        <v>83160.051904500011</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11">
+        <f>SUM(D5*B5+B6*D6+B7*D7+B8*D8)</f>
+        <v>5037.8658692978734</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -16734,7 +16899,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96CB1107-551A-4401-A108-C4996FB8D590}">
   <dimension ref="A1:AI90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+    <sheetView topLeftCell="K1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="AJ1" sqref="AJ1:AO1048576"/>
     </sheetView>
@@ -52032,8 +52197,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{465044A0-2557-4FC4-8230-2D5F5E941F36}">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="B4:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Costs Transmission and Distribution
</commit_message>
<xml_diff>
--- a/CreateBaseDeck/ExcelUserData/UserData.xlsx
+++ b/CreateBaseDeck/ExcelUserData/UserData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Remote\Desktop\Projects\TemoaHurricane_OEA\TEMOA_GIT\TemoaHurricane_V2\CreateBaseDeck\ExcelUserData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D00C178-D6BE-44A7-92D5-220AA58B1E02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B10A7550-40F4-499D-87C1-2564B48C3CB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="935" firstSheet="3" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="935" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="technologies" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <sheet name="ReadMe" sheetId="12" r:id="rId10"/>
     <sheet name="HydroPlantsNC" sheetId="13" r:id="rId11"/>
     <sheet name="DemandCalculations" sheetId="3" r:id="rId12"/>
-    <sheet name="Transmission" sheetId="18" r:id="rId13"/>
+    <sheet name="TransmissionCalculations" sheetId="18" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3231" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3295" uniqueCount="397">
   <si>
     <t>tech</t>
   </si>
@@ -1229,20 +1229,51 @@
     <t>Investment Cost [$/MW-Mile]</t>
   </si>
   <si>
-    <t>Total Energy
- Demand NC [PJ]</t>
+    <t>44-69</t>
   </si>
   <si>
-    <t>Total Energy
- Demand DEP+DEC [PJ]</t>
+    <t>closely in accordance with Regional Energy Deployment System (ReEDS) Model Documentation: Version 2018 values (Map of spur-line transmission costs)</t>
   </si>
   <si>
-    <t>Average
- Transmission Cost  [$/MW-Mile]</t>
+    <t xml:space="preserve">Average Transmission Cost from: </t>
   </si>
   <si>
-    <t>Average
- Transmission Cost  [$/MW]</t>
+    <t>Carbon Plan (2022) Appendix P | Transmission System Planning and Grid Transformation (DOE says 0.19~5.29 $/Mwh-year) National trasnmission needs study</t>
+  </si>
+  <si>
+    <t>Interregion
+ Transmission Cost  [$/MW-Mile]-2022</t>
+  </si>
+  <si>
+    <t>Transmission_Interregional</t>
+  </si>
+  <si>
+    <t>Distribution</t>
+  </si>
+  <si>
+    <t>Transmission between two different regions in NC (eg. R1&gt;R2)</t>
+  </si>
+  <si>
+    <t>Transmission inside the same region on NC (eg. R1&gt;R1)</t>
+  </si>
+  <si>
+    <t>Transmission_Regional</t>
+  </si>
+  <si>
+    <t>https://ftp.puc.texas.gov/public/puct-info/industry/electric/reports/infra/utlity_infrastructure_upgrades_rpt.pdf</t>
+  </si>
+  <si>
+    <t>Modified Automatically from the Code (Values on the right are Default Value)</t>
+  </si>
+  <si>
+    <t>Regional
+ Transmission Cost  [$/kW]-2022</t>
+  </si>
+  <si>
+    <t>Obs</t>
+  </si>
+  <si>
+    <t>Intraregional transmission have it own regional representation set all to one</t>
   </si>
 </sst>
 </file>
@@ -2997,11 +3028,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E57"/>
+  <dimension ref="A1:E60"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:A57"/>
+      <selection pane="bottomLeft" activeCell="A58" sqref="A58:A60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3850,6 +3881,48 @@
       </c>
       <c r="D57" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" t="s">
+        <v>387</v>
+      </c>
+      <c r="B58" t="s">
+        <v>24</v>
+      </c>
+      <c r="C58" t="s">
+        <v>25</v>
+      </c>
+      <c r="D58" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" t="s">
+        <v>391</v>
+      </c>
+      <c r="B59" t="s">
+        <v>24</v>
+      </c>
+      <c r="C59" t="s">
+        <v>25</v>
+      </c>
+      <c r="D59" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" t="s">
+        <v>388</v>
+      </c>
+      <c r="B60" t="s">
+        <v>24</v>
+      </c>
+      <c r="C60" t="s">
+        <v>25</v>
+      </c>
+      <c r="D60" t="s">
+        <v>388</v>
       </c>
     </row>
   </sheetData>
@@ -5361,16 +5434,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F425B7AA-21D1-411D-A9AF-54EA873F398D}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+    <col min="1" max="1" width="18" customWidth="1"/>
     <col min="2" max="2" width="16.28515625" customWidth="1"/>
     <col min="3" max="3" width="19.140625" customWidth="1"/>
     <col min="4" max="4" width="24" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -5383,6 +5458,11 @@
         <v>377</v>
       </c>
     </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>384</v>
+      </c>
+    </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>376</v>
@@ -5398,19 +5478,20 @@
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5">
-        <v>69</v>
+      <c r="A5" t="s">
+        <v>382</v>
       </c>
       <c r="B5">
         <f>5941.27*1.55</f>
         <v>9208.9685000000009</v>
       </c>
       <c r="C5">
-        <v>133</v>
+        <f>2752+133</f>
+        <v>2885</v>
       </c>
       <c r="D5">
         <f>C5/SUM($C$5:$C$8)</f>
-        <v>8.057187859695886E-3</v>
+        <v>0.1498000934627966</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -5426,7 +5507,7 @@
       </c>
       <c r="D6">
         <f t="shared" ref="D6:D8" si="0">C6/SUM($C$5:$C$8)</f>
-        <v>0.57048524868237716</v>
+        <v>0.48896619762189109</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -5442,7 +5523,7 @@
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>0.36887381111043799</v>
+        <v>0.31616387143673086</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -5458,44 +5539,38 @@
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>5.2583752347488945E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="42.75" customHeight="1">
+        <v>4.506983747858144E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="46.5" customHeight="1">
       <c r="A10" s="4" t="s">
-        <v>384</v>
-      </c>
-      <c r="B10" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="B10">
+        <f>SUM(D5*B5+B6*D6+B7*D7+B8*D8)</f>
+        <v>5633.8923732540625</v>
+      </c>
+      <c r="C10" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="43.5" customHeight="1">
+      <c r="A11" s="4" t="s">
+        <v>394</v>
+      </c>
+      <c r="B11">
+        <v>170</v>
+      </c>
+      <c r="C11" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
-      <c r="A11">
-        <f>SUM(D5*B5+B6*D6+B7*D7+B8*D8)</f>
-        <v>5037.8658692978734</v>
-      </c>
-      <c r="B11">
-        <f>B14/B13*(C5*B5+C6*B6+C7*B7+C8*B8)</f>
-        <v>76126027.940772519</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="43.5" customHeight="1">
-      <c r="A13" s="4" t="s">
-        <v>383</v>
-      </c>
-      <c r="B13">
-        <f>(DemandCalculations!A13+DemandCalculations!B13)*0.0036</f>
-        <v>547.7346</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="29.25" customHeight="1">
-      <c r="A14" s="4" t="s">
-        <v>382</v>
-      </c>
-      <c r="B14">
-        <f>Demand!B4</f>
-        <v>501.40492350355947</v>
-      </c>
+    <row r="12" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="13" spans="1:4" ht="29.25" customHeight="1">
+      <c r="A13" s="4"/>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5505,11 +5580,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A32AD897-F683-4767-9F8A-BBAC538730FF}">
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2:D34"/>
+      <selection pane="bottomLeft" activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5517,6 +5592,7 @@
     <col min="1" max="1" width="28.42578125" customWidth="1"/>
     <col min="2" max="4" width="14.5703125" customWidth="1"/>
     <col min="5" max="5" width="112.85546875" customWidth="1"/>
+    <col min="6" max="8" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -5532,7 +5608,9 @@
       <c r="D1" s="1" t="s">
         <v>373</v>
       </c>
-      <c r="E1" s="1"/>
+      <c r="E1" s="1" t="s">
+        <v>395</v>
+      </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
@@ -5968,7 +6046,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:5">
       <c r="A33" t="s">
         <v>216</v>
       </c>
@@ -5982,7 +6060,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:5">
       <c r="A34" t="s">
         <v>228</v>
       </c>
@@ -5993,6 +6071,51 @@
         <v>1</v>
       </c>
       <c r="D34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" t="s">
+        <v>387</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" t="s">
+        <v>391</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" t="s">
+        <v>388</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="D37">
         <v>1</v>
       </c>
     </row>
@@ -6004,11 +6127,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C008AD2-9FC6-4B50-8E5B-D9A0AF2799B1}">
-  <dimension ref="A1:E61"/>
+  <dimension ref="A1:E64"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D53" sqref="D53"/>
+      <selection pane="bottomLeft" activeCell="B63" sqref="B63:B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7056,6 +7179,57 @@
         <v>369</v>
       </c>
     </row>
+    <row r="62" spans="1:5">
+      <c r="A62" t="s">
+        <v>387</v>
+      </c>
+      <c r="B62">
+        <v>60</v>
+      </c>
+      <c r="C62">
+        <v>20</v>
+      </c>
+      <c r="D62" t="s">
+        <v>389</v>
+      </c>
+      <c r="E62" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" t="s">
+        <v>391</v>
+      </c>
+      <c r="B63">
+        <v>60</v>
+      </c>
+      <c r="C63">
+        <v>20</v>
+      </c>
+      <c r="D63" t="s">
+        <v>390</v>
+      </c>
+      <c r="E63" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" t="s">
+        <v>388</v>
+      </c>
+      <c r="B64">
+        <v>60</v>
+      </c>
+      <c r="C64">
+        <v>20</v>
+      </c>
+      <c r="D64" t="s">
+        <v>388</v>
+      </c>
+      <c r="E64" t="s">
+        <v>392</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7068,8 +7242,8 @@
   <dimension ref="A1:K124"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L1" sqref="L1:L1048576"/>
+      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A124" sqref="A124:K124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -11434,7 +11608,7 @@
   <sheetViews>
     <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G30" sqref="G30"/>
+      <selection pane="bottomLeft" activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -16913,11 +17087,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96CB1107-551A-4401-A108-C4996FB8D590}">
-  <dimension ref="A1:AI90"/>
+  <dimension ref="A1:AI93"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AJ1" sqref="AJ1:AO1048576"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D93" sqref="D93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -16925,7 +17099,7 @@
     <col min="1" max="1" width="12.5703125" style="6" customWidth="1"/>
     <col min="2" max="2" width="20.28515625" style="6" customWidth="1"/>
     <col min="3" max="3" width="6.85546875" style="6" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" style="6" customWidth="1"/>
     <col min="5" max="35" width="6.42578125" style="7" customWidth="1"/>
     <col min="36" max="16384" width="9.140625" style="6"/>
   </cols>
@@ -26558,6 +26732,327 @@
       </c>
       <c r="AI90" s="7">
         <v>2011</v>
+      </c>
+    </row>
+    <row r="91" spans="1:35">
+      <c r="A91" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B91" s="6" t="s">
+        <v>387</v>
+      </c>
+      <c r="C91" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D91" s="6" t="s">
+        <v>393</v>
+      </c>
+      <c r="E91" s="7">
+        <v>0</v>
+      </c>
+      <c r="F91" s="7">
+        <v>0</v>
+      </c>
+      <c r="G91" s="7">
+        <v>0</v>
+      </c>
+      <c r="H91" s="7">
+        <v>0</v>
+      </c>
+      <c r="I91" s="7">
+        <v>0</v>
+      </c>
+      <c r="J91" s="7">
+        <v>0</v>
+      </c>
+      <c r="K91" s="7">
+        <v>0</v>
+      </c>
+      <c r="L91" s="7">
+        <v>0</v>
+      </c>
+      <c r="M91" s="7">
+        <v>0</v>
+      </c>
+      <c r="N91" s="7">
+        <v>0</v>
+      </c>
+      <c r="O91" s="7">
+        <v>0</v>
+      </c>
+      <c r="P91" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q91" s="7">
+        <v>0</v>
+      </c>
+      <c r="R91" s="7">
+        <v>0</v>
+      </c>
+      <c r="S91" s="7">
+        <v>0</v>
+      </c>
+      <c r="T91" s="7">
+        <v>0</v>
+      </c>
+      <c r="U91" s="7">
+        <v>0</v>
+      </c>
+      <c r="V91" s="7">
+        <v>0</v>
+      </c>
+      <c r="W91" s="7">
+        <v>0</v>
+      </c>
+      <c r="X91" s="7">
+        <v>0</v>
+      </c>
+      <c r="Y91" s="7">
+        <v>0</v>
+      </c>
+      <c r="Z91" s="7">
+        <v>0</v>
+      </c>
+      <c r="AA91" s="7">
+        <v>0</v>
+      </c>
+      <c r="AB91" s="7">
+        <v>0</v>
+      </c>
+      <c r="AC91" s="7">
+        <v>0</v>
+      </c>
+      <c r="AD91" s="7">
+        <v>0</v>
+      </c>
+      <c r="AE91" s="7">
+        <v>0</v>
+      </c>
+      <c r="AF91" s="7">
+        <v>0</v>
+      </c>
+      <c r="AG91" s="7">
+        <v>0</v>
+      </c>
+      <c r="AH91" s="7">
+        <v>0</v>
+      </c>
+      <c r="AI91" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:35">
+      <c r="A92" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B92" s="6" t="s">
+        <v>391</v>
+      </c>
+      <c r="C92" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D92" s="6" t="s">
+        <v>393</v>
+      </c>
+      <c r="E92" s="7">
+        <v>0</v>
+      </c>
+      <c r="F92" s="7">
+        <v>0</v>
+      </c>
+      <c r="G92" s="7">
+        <v>0</v>
+      </c>
+      <c r="H92" s="7">
+        <v>0</v>
+      </c>
+      <c r="I92" s="7">
+        <v>0</v>
+      </c>
+      <c r="J92" s="7">
+        <v>0</v>
+      </c>
+      <c r="K92" s="7">
+        <v>0</v>
+      </c>
+      <c r="L92" s="7">
+        <v>0</v>
+      </c>
+      <c r="M92" s="7">
+        <v>0</v>
+      </c>
+      <c r="N92" s="7">
+        <v>0</v>
+      </c>
+      <c r="O92" s="7">
+        <v>0</v>
+      </c>
+      <c r="P92" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q92" s="7">
+        <v>0</v>
+      </c>
+      <c r="R92" s="7">
+        <v>0</v>
+      </c>
+      <c r="S92" s="7">
+        <v>0</v>
+      </c>
+      <c r="T92" s="7">
+        <v>0</v>
+      </c>
+      <c r="U92" s="7">
+        <v>0</v>
+      </c>
+      <c r="V92" s="7">
+        <v>0</v>
+      </c>
+      <c r="W92" s="7">
+        <v>0</v>
+      </c>
+      <c r="X92" s="7">
+        <v>0</v>
+      </c>
+      <c r="Y92" s="7">
+        <v>0</v>
+      </c>
+      <c r="Z92" s="7">
+        <v>0</v>
+      </c>
+      <c r="AA92" s="7">
+        <v>0</v>
+      </c>
+      <c r="AB92" s="7">
+        <v>0</v>
+      </c>
+      <c r="AC92" s="7">
+        <v>0</v>
+      </c>
+      <c r="AD92" s="7">
+        <v>0</v>
+      </c>
+      <c r="AE92" s="7">
+        <v>0</v>
+      </c>
+      <c r="AF92" s="7">
+        <v>0</v>
+      </c>
+      <c r="AG92" s="7">
+        <v>0</v>
+      </c>
+      <c r="AH92" s="7">
+        <v>0</v>
+      </c>
+      <c r="AI92" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:35">
+      <c r="A93" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B93" s="6" t="s">
+        <v>388</v>
+      </c>
+      <c r="C93" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D93" s="6" t="s">
+        <v>393</v>
+      </c>
+      <c r="E93" s="7">
+        <v>0</v>
+      </c>
+      <c r="F93" s="7">
+        <v>0</v>
+      </c>
+      <c r="G93" s="7">
+        <v>0</v>
+      </c>
+      <c r="H93" s="7">
+        <v>0</v>
+      </c>
+      <c r="I93" s="7">
+        <v>0</v>
+      </c>
+      <c r="J93" s="7">
+        <v>0</v>
+      </c>
+      <c r="K93" s="7">
+        <v>0</v>
+      </c>
+      <c r="L93" s="7">
+        <v>0</v>
+      </c>
+      <c r="M93" s="7">
+        <v>0</v>
+      </c>
+      <c r="N93" s="7">
+        <v>0</v>
+      </c>
+      <c r="O93" s="7">
+        <v>0</v>
+      </c>
+      <c r="P93" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q93" s="7">
+        <v>0</v>
+      </c>
+      <c r="R93" s="7">
+        <v>0</v>
+      </c>
+      <c r="S93" s="7">
+        <v>0</v>
+      </c>
+      <c r="T93" s="7">
+        <v>0</v>
+      </c>
+      <c r="U93" s="7">
+        <v>0</v>
+      </c>
+      <c r="V93" s="7">
+        <v>0</v>
+      </c>
+      <c r="W93" s="7">
+        <v>0</v>
+      </c>
+      <c r="X93" s="7">
+        <v>0</v>
+      </c>
+      <c r="Y93" s="7">
+        <v>0</v>
+      </c>
+      <c r="Z93" s="7">
+        <v>0</v>
+      </c>
+      <c r="AA93" s="7">
+        <v>0</v>
+      </c>
+      <c r="AB93" s="7">
+        <v>0</v>
+      </c>
+      <c r="AC93" s="7">
+        <v>0</v>
+      </c>
+      <c r="AD93" s="7">
+        <v>0</v>
+      </c>
+      <c r="AE93" s="7">
+        <v>0</v>
+      </c>
+      <c r="AF93" s="7">
+        <v>0</v>
+      </c>
+      <c r="AG93" s="7">
+        <v>0</v>
+      </c>
+      <c r="AH93" s="7">
+        <v>0</v>
+      </c>
+      <c r="AI93" s="7">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -26569,11 +27064,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CD5D24F-D6D8-45F0-9B18-7F7BBE5186DB}">
-  <dimension ref="A1:AI119"/>
+  <dimension ref="A1:AI122"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AJ1" sqref="AJ1:AO1048576"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A91" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C120" sqref="C120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -39319,6 +39814,327 @@
         <v>17.82</v>
       </c>
     </row>
+    <row r="120" spans="1:35">
+      <c r="A120" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B120" s="6" t="s">
+        <v>387</v>
+      </c>
+      <c r="C120" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D120" s="6" t="s">
+        <v>393</v>
+      </c>
+      <c r="E120" s="7">
+        <v>0</v>
+      </c>
+      <c r="F120" s="7">
+        <v>0</v>
+      </c>
+      <c r="G120" s="7">
+        <v>0</v>
+      </c>
+      <c r="H120" s="7">
+        <v>0</v>
+      </c>
+      <c r="I120" s="7">
+        <v>0</v>
+      </c>
+      <c r="J120" s="7">
+        <v>0</v>
+      </c>
+      <c r="K120" s="7">
+        <v>0</v>
+      </c>
+      <c r="L120" s="7">
+        <v>0</v>
+      </c>
+      <c r="M120" s="7">
+        <v>0</v>
+      </c>
+      <c r="N120" s="7">
+        <v>0</v>
+      </c>
+      <c r="O120" s="7">
+        <v>0</v>
+      </c>
+      <c r="P120" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q120" s="7">
+        <v>0</v>
+      </c>
+      <c r="R120" s="7">
+        <v>0</v>
+      </c>
+      <c r="S120" s="7">
+        <v>0</v>
+      </c>
+      <c r="T120" s="7">
+        <v>0</v>
+      </c>
+      <c r="U120" s="7">
+        <v>0</v>
+      </c>
+      <c r="V120" s="7">
+        <v>0</v>
+      </c>
+      <c r="W120" s="7">
+        <v>0</v>
+      </c>
+      <c r="X120" s="7">
+        <v>0</v>
+      </c>
+      <c r="Y120" s="7">
+        <v>0</v>
+      </c>
+      <c r="Z120" s="7">
+        <v>0</v>
+      </c>
+      <c r="AA120" s="7">
+        <v>0</v>
+      </c>
+      <c r="AB120" s="7">
+        <v>0</v>
+      </c>
+      <c r="AC120" s="7">
+        <v>0</v>
+      </c>
+      <c r="AD120" s="7">
+        <v>0</v>
+      </c>
+      <c r="AE120" s="7">
+        <v>0</v>
+      </c>
+      <c r="AF120" s="7">
+        <v>0</v>
+      </c>
+      <c r="AG120" s="7">
+        <v>0</v>
+      </c>
+      <c r="AH120" s="7">
+        <v>0</v>
+      </c>
+      <c r="AI120" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:35">
+      <c r="A121" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B121" s="6" t="s">
+        <v>391</v>
+      </c>
+      <c r="C121" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D121" s="6" t="s">
+        <v>393</v>
+      </c>
+      <c r="E121" s="7">
+        <v>0</v>
+      </c>
+      <c r="F121" s="7">
+        <v>0</v>
+      </c>
+      <c r="G121" s="7">
+        <v>0</v>
+      </c>
+      <c r="H121" s="7">
+        <v>0</v>
+      </c>
+      <c r="I121" s="7">
+        <v>0</v>
+      </c>
+      <c r="J121" s="7">
+        <v>0</v>
+      </c>
+      <c r="K121" s="7">
+        <v>0</v>
+      </c>
+      <c r="L121" s="7">
+        <v>0</v>
+      </c>
+      <c r="M121" s="7">
+        <v>0</v>
+      </c>
+      <c r="N121" s="7">
+        <v>0</v>
+      </c>
+      <c r="O121" s="7">
+        <v>0</v>
+      </c>
+      <c r="P121" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q121" s="7">
+        <v>0</v>
+      </c>
+      <c r="R121" s="7">
+        <v>0</v>
+      </c>
+      <c r="S121" s="7">
+        <v>0</v>
+      </c>
+      <c r="T121" s="7">
+        <v>0</v>
+      </c>
+      <c r="U121" s="7">
+        <v>0</v>
+      </c>
+      <c r="V121" s="7">
+        <v>0</v>
+      </c>
+      <c r="W121" s="7">
+        <v>0</v>
+      </c>
+      <c r="X121" s="7">
+        <v>0</v>
+      </c>
+      <c r="Y121" s="7">
+        <v>0</v>
+      </c>
+      <c r="Z121" s="7">
+        <v>0</v>
+      </c>
+      <c r="AA121" s="7">
+        <v>0</v>
+      </c>
+      <c r="AB121" s="7">
+        <v>0</v>
+      </c>
+      <c r="AC121" s="7">
+        <v>0</v>
+      </c>
+      <c r="AD121" s="7">
+        <v>0</v>
+      </c>
+      <c r="AE121" s="7">
+        <v>0</v>
+      </c>
+      <c r="AF121" s="7">
+        <v>0</v>
+      </c>
+      <c r="AG121" s="7">
+        <v>0</v>
+      </c>
+      <c r="AH121" s="7">
+        <v>0</v>
+      </c>
+      <c r="AI121" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:35">
+      <c r="A122" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B122" s="6" t="s">
+        <v>388</v>
+      </c>
+      <c r="C122" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D122" s="6" t="s">
+        <v>393</v>
+      </c>
+      <c r="E122" s="7">
+        <v>0</v>
+      </c>
+      <c r="F122" s="7">
+        <v>0</v>
+      </c>
+      <c r="G122" s="7">
+        <v>0</v>
+      </c>
+      <c r="H122" s="7">
+        <v>0</v>
+      </c>
+      <c r="I122" s="7">
+        <v>0</v>
+      </c>
+      <c r="J122" s="7">
+        <v>0</v>
+      </c>
+      <c r="K122" s="7">
+        <v>0</v>
+      </c>
+      <c r="L122" s="7">
+        <v>0</v>
+      </c>
+      <c r="M122" s="7">
+        <v>0</v>
+      </c>
+      <c r="N122" s="7">
+        <v>0</v>
+      </c>
+      <c r="O122" s="7">
+        <v>0</v>
+      </c>
+      <c r="P122" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q122" s="7">
+        <v>0</v>
+      </c>
+      <c r="R122" s="7">
+        <v>0</v>
+      </c>
+      <c r="S122" s="7">
+        <v>0</v>
+      </c>
+      <c r="T122" s="7">
+        <v>0</v>
+      </c>
+      <c r="U122" s="7">
+        <v>0</v>
+      </c>
+      <c r="V122" s="7">
+        <v>0</v>
+      </c>
+      <c r="W122" s="7">
+        <v>0</v>
+      </c>
+      <c r="X122" s="7">
+        <v>0</v>
+      </c>
+      <c r="Y122" s="7">
+        <v>0</v>
+      </c>
+      <c r="Z122" s="7">
+        <v>0</v>
+      </c>
+      <c r="AA122" s="7">
+        <v>0</v>
+      </c>
+      <c r="AB122" s="7">
+        <v>0</v>
+      </c>
+      <c r="AC122" s="7">
+        <v>0</v>
+      </c>
+      <c r="AD122" s="7">
+        <v>0</v>
+      </c>
+      <c r="AE122" s="7">
+        <v>0</v>
+      </c>
+      <c r="AF122" s="7">
+        <v>0</v>
+      </c>
+      <c r="AG122" s="7">
+        <v>0</v>
+      </c>
+      <c r="AH122" s="7">
+        <v>0</v>
+      </c>
+      <c r="AI122" s="7">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -39328,11 +40144,11 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1F64963-0CDD-4BE6-B0AC-E6FD0D7CCBEC}">
-  <dimension ref="A1:AI119"/>
+  <dimension ref="A1:AI122"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AJ1" sqref="AJ1:AQ1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A97" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B120" sqref="B120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -52200,6 +53016,327 @@
       </c>
       <c r="AI119" s="7">
         <v>0.51300000000000001</v>
+      </c>
+    </row>
+    <row r="120" spans="1:35">
+      <c r="A120" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B120" s="6" t="s">
+        <v>387</v>
+      </c>
+      <c r="C120" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D120" s="6" t="s">
+        <v>393</v>
+      </c>
+      <c r="E120" s="7">
+        <v>0</v>
+      </c>
+      <c r="F120" s="7">
+        <v>0</v>
+      </c>
+      <c r="G120" s="7">
+        <v>0</v>
+      </c>
+      <c r="H120" s="7">
+        <v>0</v>
+      </c>
+      <c r="I120" s="7">
+        <v>0</v>
+      </c>
+      <c r="J120" s="7">
+        <v>0</v>
+      </c>
+      <c r="K120" s="7">
+        <v>0</v>
+      </c>
+      <c r="L120" s="7">
+        <v>0</v>
+      </c>
+      <c r="M120" s="7">
+        <v>0</v>
+      </c>
+      <c r="N120" s="7">
+        <v>0</v>
+      </c>
+      <c r="O120" s="7">
+        <v>0</v>
+      </c>
+      <c r="P120" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q120" s="7">
+        <v>0</v>
+      </c>
+      <c r="R120" s="7">
+        <v>0</v>
+      </c>
+      <c r="S120" s="7">
+        <v>0</v>
+      </c>
+      <c r="T120" s="7">
+        <v>0</v>
+      </c>
+      <c r="U120" s="7">
+        <v>0</v>
+      </c>
+      <c r="V120" s="7">
+        <v>0</v>
+      </c>
+      <c r="W120" s="7">
+        <v>0</v>
+      </c>
+      <c r="X120" s="7">
+        <v>0</v>
+      </c>
+      <c r="Y120" s="7">
+        <v>0</v>
+      </c>
+      <c r="Z120" s="7">
+        <v>0</v>
+      </c>
+      <c r="AA120" s="7">
+        <v>0</v>
+      </c>
+      <c r="AB120" s="7">
+        <v>0</v>
+      </c>
+      <c r="AC120" s="7">
+        <v>0</v>
+      </c>
+      <c r="AD120" s="7">
+        <v>0</v>
+      </c>
+      <c r="AE120" s="7">
+        <v>0</v>
+      </c>
+      <c r="AF120" s="7">
+        <v>0</v>
+      </c>
+      <c r="AG120" s="7">
+        <v>0</v>
+      </c>
+      <c r="AH120" s="7">
+        <v>0</v>
+      </c>
+      <c r="AI120" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:35">
+      <c r="A121" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B121" s="6" t="s">
+        <v>391</v>
+      </c>
+      <c r="C121" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D121" s="6" t="s">
+        <v>393</v>
+      </c>
+      <c r="E121" s="7">
+        <v>0</v>
+      </c>
+      <c r="F121" s="7">
+        <v>0</v>
+      </c>
+      <c r="G121" s="7">
+        <v>0</v>
+      </c>
+      <c r="H121" s="7">
+        <v>0</v>
+      </c>
+      <c r="I121" s="7">
+        <v>0</v>
+      </c>
+      <c r="J121" s="7">
+        <v>0</v>
+      </c>
+      <c r="K121" s="7">
+        <v>0</v>
+      </c>
+      <c r="L121" s="7">
+        <v>0</v>
+      </c>
+      <c r="M121" s="7">
+        <v>0</v>
+      </c>
+      <c r="N121" s="7">
+        <v>0</v>
+      </c>
+      <c r="O121" s="7">
+        <v>0</v>
+      </c>
+      <c r="P121" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q121" s="7">
+        <v>0</v>
+      </c>
+      <c r="R121" s="7">
+        <v>0</v>
+      </c>
+      <c r="S121" s="7">
+        <v>0</v>
+      </c>
+      <c r="T121" s="7">
+        <v>0</v>
+      </c>
+      <c r="U121" s="7">
+        <v>0</v>
+      </c>
+      <c r="V121" s="7">
+        <v>0</v>
+      </c>
+      <c r="W121" s="7">
+        <v>0</v>
+      </c>
+      <c r="X121" s="7">
+        <v>0</v>
+      </c>
+      <c r="Y121" s="7">
+        <v>0</v>
+      </c>
+      <c r="Z121" s="7">
+        <v>0</v>
+      </c>
+      <c r="AA121" s="7">
+        <v>0</v>
+      </c>
+      <c r="AB121" s="7">
+        <v>0</v>
+      </c>
+      <c r="AC121" s="7">
+        <v>0</v>
+      </c>
+      <c r="AD121" s="7">
+        <v>0</v>
+      </c>
+      <c r="AE121" s="7">
+        <v>0</v>
+      </c>
+      <c r="AF121" s="7">
+        <v>0</v>
+      </c>
+      <c r="AG121" s="7">
+        <v>0</v>
+      </c>
+      <c r="AH121" s="7">
+        <v>0</v>
+      </c>
+      <c r="AI121" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:35">
+      <c r="A122" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B122" s="6" t="s">
+        <v>388</v>
+      </c>
+      <c r="C122" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D122" s="6" t="s">
+        <v>393</v>
+      </c>
+      <c r="E122" s="7">
+        <v>0</v>
+      </c>
+      <c r="F122" s="7">
+        <v>0</v>
+      </c>
+      <c r="G122" s="7">
+        <v>0</v>
+      </c>
+      <c r="H122" s="7">
+        <v>0</v>
+      </c>
+      <c r="I122" s="7">
+        <v>0</v>
+      </c>
+      <c r="J122" s="7">
+        <v>0</v>
+      </c>
+      <c r="K122" s="7">
+        <v>0</v>
+      </c>
+      <c r="L122" s="7">
+        <v>0</v>
+      </c>
+      <c r="M122" s="7">
+        <v>0</v>
+      </c>
+      <c r="N122" s="7">
+        <v>0</v>
+      </c>
+      <c r="O122" s="7">
+        <v>0</v>
+      </c>
+      <c r="P122" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q122" s="7">
+        <v>0</v>
+      </c>
+      <c r="R122" s="7">
+        <v>0</v>
+      </c>
+      <c r="S122" s="7">
+        <v>0</v>
+      </c>
+      <c r="T122" s="7">
+        <v>0</v>
+      </c>
+      <c r="U122" s="7">
+        <v>0</v>
+      </c>
+      <c r="V122" s="7">
+        <v>0</v>
+      </c>
+      <c r="W122" s="7">
+        <v>0</v>
+      </c>
+      <c r="X122" s="7">
+        <v>0</v>
+      </c>
+      <c r="Y122" s="7">
+        <v>0</v>
+      </c>
+      <c r="Z122" s="7">
+        <v>0</v>
+      </c>
+      <c r="AA122" s="7">
+        <v>0</v>
+      </c>
+      <c r="AB122" s="7">
+        <v>0</v>
+      </c>
+      <c r="AC122" s="7">
+        <v>0</v>
+      </c>
+      <c r="AD122" s="7">
+        <v>0</v>
+      </c>
+      <c r="AE122" s="7">
+        <v>0</v>
+      </c>
+      <c r="AF122" s="7">
+        <v>0</v>
+      </c>
+      <c r="AG122" s="7">
+        <v>0</v>
+      </c>
+      <c r="AH122" s="7">
+        <v>0</v>
+      </c>
+      <c r="AI122" s="7">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>